<commit_message>
Added more notes to spreadsheet
</commit_message>
<xml_diff>
--- a/tests/test01/Unit2 Notes.xlsx
+++ b/tests/test01/Unit2 Notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul_\OneDrive - Edinburgh Napier University\eSecurity\Labs\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul_\source\repos\40448091\eSecurity\tests\test01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="148">
   <si>
     <t>RC2</t>
   </si>
@@ -163,9 +163,6 @@
     <t xml:space="preserve">Rivest ciper, replaces DES, 40 to 128 bit keys (increments of 8 bits), 40 bit easily crackable. </t>
   </si>
   <si>
-    <t xml:space="preserve">Rijndael, </t>
-  </si>
-  <si>
     <t>128 bit blocks, 128,192,256 bit encryption keys</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
   </si>
   <si>
     <t>256 bit key / 128 bit + 32 bit nonce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This creates a key stream, which is then XORed with the plaintext stream. In software, it is more than three times faster than AES, and is well suited to lower-powered devices and in real-time communications. ChaCha operates on 32-bit bits with a key of 256 bits </t>
   </si>
   <si>
     <t xml:space="preserve">Unsafe because identical input blocks produce identical output. </t>
@@ -256,18 +250,9 @@
     <t>print "NT Hash:"+passlib.hash.nthash.encrypt(string)</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>python AES.py</t>
   </si>
   <si>
-    <t>DHE-RSA Ephemeral Diffee-Hellman Key Exchange</t>
-  </si>
-  <si>
-    <t>DH Diffee-Hellman Key Exchange</t>
-  </si>
-  <si>
     <t>HMAC</t>
   </si>
   <si>
@@ -289,9 +274,6 @@
     <t>L2 Slide 31</t>
   </si>
   <si>
-    <t>L2 Slide 41</t>
-  </si>
-  <si>
     <t>Hash</t>
   </si>
   <si>
@@ -302,6 +284,212 @@
   </si>
   <si>
     <t>python PBKDF2.py</t>
+  </si>
+  <si>
+    <t>Rijndael, Rounds= Add round key, Substitite, Shift rows, Mix columns (X 10, 12, 14 depending on key size)</t>
+  </si>
+  <si>
+    <t>ECDH</t>
+  </si>
+  <si>
+    <t>Elliptic Curve DH</t>
+  </si>
+  <si>
+    <t>Diffee-Hellman (DH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DHE-RSA </t>
+  </si>
+  <si>
+    <t>Ephemeral DH</t>
+  </si>
+  <si>
+    <t>L5 Slide 13</t>
+  </si>
+  <si>
+    <t>L5 Slide 9</t>
+  </si>
+  <si>
+    <t>DH Generator</t>
+  </si>
+  <si>
+    <t>L5 Slide 15</t>
+  </si>
+  <si>
+    <t>Y = Gx mod p</t>
+  </si>
+  <si>
+    <t>• DH Group 5: 1,536 bit prime. 
+• DH Group 2: 1,024 bit prime. 
+• DH Group 1: 768-bit prime.
+ Weaknesses 
+• Imperfect Forward Secrecy – fairly easy to precompute on values for two popular DH parameters (and which use the DHE_EXPORT cipher set).  
+• research found that one was used as a default in the around 7% of the Top 1 million web sites and was hard coded into the Apache httpd service. Overall, at the time, it was found that over 3% of Web sites were still using the default.</t>
+  </si>
+  <si>
+    <t>L5 Slide 21, 23</t>
+  </si>
+  <si>
+    <t>Curve 25519 == (ie. (2^255)-19)
+G=Generator, p=public key, gradient = private key
+Even if Generator, curve &amp; public key are know, it's difficult to calculate value for Private key in Polynomial Computing time</t>
+  </si>
+  <si>
+    <t>Public Key Exchange</t>
+  </si>
+  <si>
+    <t>* Bob creates private (session) key and encrypts with Alice's public key
+* Alice decrypts with her private key</t>
+  </si>
+  <si>
+    <t>L5 Slide 21, 28</t>
+  </si>
+  <si>
+    <t>Trusted Infrastructure</t>
+  </si>
+  <si>
+    <t>L5 Slide 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This creates a key stream, which is then XORed with the plaintext stream. In software, it is more than three times faster than AES, and is well suited to lower-powered devices and in real-time communications. ChaCha operates on 32-bit bits with a key of 256 bits 
+</t>
+  </si>
+  <si>
+    <t>SHA-1</t>
+  </si>
+  <si>
+    <t>128 bit sig</t>
+  </si>
+  <si>
+    <t>L3 Slide 4</t>
+  </si>
+  <si>
+    <t>160 bit sig</t>
+  </si>
+  <si>
+    <t>Bcrypt</t>
+  </si>
+  <si>
+    <t>Hash with salt</t>
+  </si>
+  <si>
+    <t>LM Hash</t>
+  </si>
+  <si>
+    <t>Windows, less than 15 chars long</t>
+  </si>
+  <si>
+    <t>L3 Slide 15</t>
+  </si>
+  <si>
+    <t>Tiger, RIPEMED, SHA-3</t>
+  </si>
+  <si>
+    <t>Murmur, FNV</t>
+  </si>
+  <si>
+    <t>L3 Slide 16</t>
+  </si>
+  <si>
+    <t>Password + Salt + desired key Len</t>
+  </si>
+  <si>
+    <t>L3 Slide 17</t>
+  </si>
+  <si>
+    <t>L3 Slide 21</t>
+  </si>
+  <si>
+    <t>Collisions</t>
+  </si>
+  <si>
+    <t>Hash Collisions</t>
+  </si>
+  <si>
+    <t>L3 Slide 23</t>
+  </si>
+  <si>
+    <t>NT Hash (MD4), LM, NT LM</t>
+  </si>
+  <si>
+    <t>L3 Slide 27</t>
+  </si>
+  <si>
+    <t>Hackers Crackers Miners</t>
+  </si>
+  <si>
+    <t>Terrahash</t>
+  </si>
+  <si>
+    <t>L3 Slide 32</t>
+  </si>
+  <si>
+    <t>L3 Slide 36</t>
+  </si>
+  <si>
+    <t>Hash of message, Encrypted with SECRET key</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>One Time Password</t>
+  </si>
+  <si>
+    <t>Time / counter based</t>
+  </si>
+  <si>
+    <t>L3 Slide 38</t>
+  </si>
+  <si>
+    <t>HashCat</t>
+  </si>
+  <si>
+    <t>Cheat Sheet</t>
+  </si>
+  <si>
+    <t>Open SSL</t>
+  </si>
+  <si>
+    <t>OpenSSL.txt</t>
+  </si>
+  <si>
+    <t>L3 Slide 41, 57</t>
+  </si>
+  <si>
+    <t>L2 Slide 21</t>
+  </si>
+  <si>
+    <t>Integer factorisation, digital certs, SSL
+primes p &amp; q, N(modulus) = p*q, PHI=(p-1)(q-1)
+* Select e for no common factor with PHI. e=3  : Encryption key [e,n] 
+* Select d such that (d x e) mod 20 = 1 (inverse mod) : Decryption key [d,n]</t>
+  </si>
+  <si>
+    <t>L4 Slide 18, 21, 27</t>
+  </si>
+  <si>
+    <t>L4 Slide 31, 35</t>
+  </si>
+  <si>
+    <t>L4 Slide 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Y = Gx mod P. 
+• Y = Gx mod p  
+• G is picked from cyclic group (Explained in Key Handshaking section).
+• p is a prime number. 
+• Example here.</t>
+  </si>
+  <si>
+    <t>https://asecuritysite.com/encryption/elgamal
+https://asecuritysite.com/encryption/pickg</t>
+  </si>
+  <si>
+    <t>PGP</t>
+  </si>
+  <si>
+    <t>L4 Slide 47</t>
   </si>
 </sst>
 </file>
@@ -354,18 +542,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -647,234 +844,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomRight" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>75</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G6" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" t="s">
-        <v>52</v>
+      <c r="F7" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="F8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="I8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="G9" s="4"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="G10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
-        <v>55</v>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -882,277 +1099,551 @@
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" t="s">
-        <v>87</v>
+      <c r="A14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>87</v>
+      <c r="A15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>123</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
+      <c r="A18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
+      <c r="A19" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
+      <c r="A20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
+      <c r="A21" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
+      <c r="A22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
+      <c r="G23" s="4"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" t="s">
-        <v>53</v>
+      <c r="A26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>63</v>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>58</v>
+      <c r="A31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="I33" s="4"/>
+      <c r="A33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>61</v>
-      </c>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>62</v>
+      <c r="A35" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>90</v>
-      </c>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I39" s="4"/>
+      <c r="A39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" ht="186" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F54" s="5"/>
+      <c r="G54" s="4"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>79</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I46" s="4"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I47" s="4"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I48" s="4"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I49" s="4"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I50" s="4"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I51" s="4"/>
-    </row>
-    <row r="52" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="B61" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I52" s="4"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>73</v>
-      </c>
-      <c r="F53" t="s">
-        <v>74</v>
-      </c>
-      <c r="I53" s="4"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G26" r:id="rId1"/>
-    <hyperlink ref="G17" r:id="rId2"/>
-    <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="G6" r:id="rId4"/>
-    <hyperlink ref="G5" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G28" r:id="rId7"/>
-    <hyperlink ref="I8" r:id="rId8"/>
-    <hyperlink ref="H37" r:id="rId9"/>
-    <hyperlink ref="I41" r:id="rId10"/>
-    <hyperlink ref="I6" r:id="rId11"/>
-    <hyperlink ref="I2:I5" r:id="rId12" display="."/>
-    <hyperlink ref="I9:I29" r:id="rId13" display="."/>
-    <hyperlink ref="I30" r:id="rId14"/>
-    <hyperlink ref="I45" r:id="rId15"/>
-    <hyperlink ref="I37" r:id="rId16" display="python DH.py"/>
+    <hyperlink ref="G35" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G7" r:id="rId5"/>
+    <hyperlink ref="I8" r:id="rId6"/>
+    <hyperlink ref="H33" r:id="rId7"/>
+    <hyperlink ref="I48" r:id="rId8"/>
+    <hyperlink ref="I6" r:id="rId9"/>
+    <hyperlink ref="I9:I38" r:id="rId10" display="."/>
+    <hyperlink ref="I39" r:id="rId11"/>
+    <hyperlink ref="I57" r:id="rId12"/>
+    <hyperlink ref="I33" r:id="rId13" display="python DH.py"/>
+    <hyperlink ref="G37" r:id="rId14" display="L2 Slide 41"/>
+    <hyperlink ref="G48" r:id="rId15" display="L2 Slide 41"/>
+    <hyperlink ref="G50" r:id="rId16" display="L2 Slide 41"/>
+    <hyperlink ref="G49" r:id="rId17" display="L2 Slide 41"/>
+    <hyperlink ref="G51" r:id="rId18" display="L2 Slide 41"/>
+    <hyperlink ref="G52" r:id="rId19" display="L2 Slide 41"/>
+    <hyperlink ref="G53" r:id="rId20" display="L2 Slide 41"/>
+    <hyperlink ref="G14" r:id="rId21" display="L2 Slide 23"/>
+    <hyperlink ref="G15" r:id="rId22" display="L2 Slide 23"/>
+    <hyperlink ref="G16" r:id="rId23" display="L2 Slide 23"/>
+    <hyperlink ref="G19" r:id="rId24" display="L2 Slide 23"/>
+    <hyperlink ref="G18" r:id="rId25" display="L2 Slide 23"/>
+    <hyperlink ref="G20" r:id="rId26" display="L2 Slide 23"/>
+    <hyperlink ref="G21" r:id="rId27" display="L2 Slide 23"/>
+    <hyperlink ref="G33" r:id="rId28"/>
+    <hyperlink ref="G39" r:id="rId29" display="L2 Slide 31"/>
+    <hyperlink ref="G22" r:id="rId30" display="L2 Slide 23"/>
+    <hyperlink ref="G17" r:id="rId31" display="L2 Slide 23"/>
+    <hyperlink ref="G55" r:id="rId32" display="L2 Slide 31"/>
+    <hyperlink ref="G57" r:id="rId33" display="L2 Slide 31"/>
+    <hyperlink ref="G58" r:id="rId34" display="L2 Slide 31"/>
+    <hyperlink ref="G64" r:id="rId35" display="L2 Slide 31"/>
+    <hyperlink ref="H64" r:id="rId36" display="conversion_table.pdf"/>
+    <hyperlink ref="H67" r:id="rId37"/>
+    <hyperlink ref="G25:G31" r:id="rId38" display="L2 Slide 23"/>
+    <hyperlink ref="H11" r:id="rId39" display="https://asecuritysite.com/encryption/elgamal"/>
+    <hyperlink ref="H69" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -1649,10 +2140,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1674,15 +2165,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A478DC777839B84AA78BE34820D6106B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2b0b78b229846a0fb540ef9e6a52c1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e77d71de-ed03-4187-81e7-c51d7bba4b52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a685b91e9f3b401c2950534508025d54" ns3:_="">
     <xsd:import namespace="e77d71de-ed03-4187-81e7-c51d7bba4b52"/>
@@ -1854,6 +2336,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1861,14 +2352,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DAA1A3C-67DD-4598-9E7E-62167BBD3C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0034C2E-083F-4678-AC72-7D9E121334AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1886,18 +2369,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DAA1A3C-67DD-4598-9E7E-62167BBD3C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35899522-1E86-4974-B69A-65376177F53F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="e77d71de-ed03-4187-81e7-c51d7bba4b52"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>